<commit_message>
Changes to be committed: 	modified:   deployment_manifests/assets_groups_manifest.csv 	modified:   "\320\270\321\201\321\205\320\276\320\264\320\275\321\213\320\265 \320\274\320\260\320\275\320\270\321\204\320\265\321\201\321\202\321\213/groups_manifest.xlsx"
</commit_message>
<xml_diff>
--- a/исходные манифесты/groups_manifest.xlsx
+++ b/исходные манифесты/groups_manifest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Кирилл\Desktop\разработка\MPVM_api_python\исходные манифесты\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.krasnovskiy\Work Folders\Desktop\development\git\PT-MP-VM-APi-Python\PT-MP-VM-Api\исходные манифесты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396D8BC3-C3F6-4EB2-A812-058F6D64463A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392AB74D-1E44-4E39-A811-3ADEE25BCFBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>DC</t>
   </si>
   <si>
-    <t>СУБД</t>
-  </si>
-  <si>
     <t>Хосты, на которых есть средства управления базами данных</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>Host.HostRoles.Role = 'DNS Server'</t>
+  </si>
+  <si>
+    <t>СУБД_2</t>
   </si>
 </sst>
 </file>
@@ -512,55 +512,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" t="s">
-        <v>48</v>
       </c>
       <c r="K1" t="s">
         <v>0</v>
@@ -584,7 +584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -613,7 +613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -642,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -656,7 +656,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -674,7 +674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -688,7 +688,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -706,7 +706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -767,7 +767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -781,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -799,7 +799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -813,7 +813,7 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -831,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -860,7 +860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -874,7 +874,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -892,7 +892,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -906,7 +906,7 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -924,12 +924,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -938,7 +938,7 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>

</xml_diff>